<commit_message>
fix: correct typo in game instructions
</commit_message>
<xml_diff>
--- a/docs/controle.xlsx
+++ b/docs/controle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelo/Meu Drive (marceloasouza52@gmail.com)/senac/oitavo-semestre/engenharia-de-software2/projeto/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263CD648-7D39-E44A-9739-840EF0EE9FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E263C7FF-ADE3-044A-A089-4A735E2C6F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" activeTab="3" xr2:uid="{E166ED89-6562-4373-A416-CC4B8503D8FA}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -560,9 +560,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3270,7 +3267,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3463,10 +3460,10 @@
       <c r="B14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="28"/>
+      <c r="D14" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="28"/>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -3476,10 +3473,10 @@
       <c r="B15" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="28"/>
+      <c r="D15" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="28"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -3489,10 +3486,10 @@
       <c r="B16" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="28"/>
+      <c r="D16" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="28"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -3502,7 +3499,7 @@
       <c r="B17" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="28" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="28"/>
@@ -3531,16 +3528,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eff2e8f5-27d7-4f61-9f93-1cf91307dac9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100754B351E8A6E7649BF30E6B840EC0436" ma:contentTypeVersion="11" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="9bbc7b9183649a6d9716a89e120180b5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eff2e8f5-27d7-4f61-9f93-1cf91307dac9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b66f89bbecccfdd766b6574b40f12ec" ns2:_="">
     <xsd:import namespace="eff2e8f5-27d7-4f61-9f93-1cf91307dac9"/>
@@ -3724,6 +3711,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eff2e8f5-27d7-4f61-9f93-1cf91307dac9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51A829F1-35C3-4A75-8FD7-FF6D25F10C80}">
   <ds:schemaRefs>
@@ -3733,16 +3730,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FA2EB68-5829-4389-86C8-A3A6F8F290CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="eff2e8f5-27d7-4f61-9f93-1cf91307dac9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{128F90C2-F667-4057-B969-511C7587B661}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3760,6 +3747,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FA2EB68-5829-4389-86C8-A3A6F8F290CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="eff2e8f5-27d7-4f61-9f93-1cf91307dac9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{5d722c75-9049-497d-aec7-8c09c4025ead}" enabled="1" method="Standard" siteId="{7da4edd9-50bb-48f7-81af-0ca98f2c9594}" contentBits="1" removed="0"/>

</xml_diff>